<commit_message>
create new branch KikaAutomator-photon
</commit_message>
<xml_diff>
--- a/testcase/case_id.xlsx
+++ b/testcase/case_id.xlsx
@@ -22,70 +22,70 @@
     <t>pool_id</t>
   </si>
   <si>
-    <t>test_InputMethod_SCB_func_01_01_01_0001</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_0002</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_0003</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_0008</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_0009</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_00010</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_00011</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_00013</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_00016</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_01_01_00036</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_02_0003</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_03_0010</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_04_0002</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_05_0005</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_05_0034</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_07_0001</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_08_0001</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_08_0005</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_08_0006</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_01_09_0002</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_02_02_02_0003</t>
-  </si>
-  <si>
-    <t>test_InputMethod_SCB_func_03_01_01_0002</t>
+    <t>test_InputMethod_SCB_Func_01_01_01_0001</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_0002</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_0003</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_0008</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_0009</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_00010</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_00011</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_00013</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_00016</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_01_01_00036</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_02_0003</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_03_0010</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_04_0002</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_05_0005</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_05_0034</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_07_0001</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_08_0001</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_08_0005</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_08_0006</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_01_09_0002</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_02_02_02_0003</t>
+  </si>
+  <si>
+    <t>test_InputMethod_SCB_Func_03_01_01_0002</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelCol="4"/>

</xml_diff>